<commit_message>
Added new procedures for email notifications
Added new procedures for email notifications
</commit_message>
<xml_diff>
--- a/Student Details_24_25.xlsx
+++ b/Student Details_24_25.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Class1B" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="LKG-A" sheetId="13" r:id="rId11"/>
     <sheet name="LKG-B" sheetId="14" r:id="rId12"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId13"/>
+    <sheet name="Sheet2" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4135" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4261" uniqueCount="831">
   <si>
     <t>S.No</t>
   </si>
@@ -2466,6 +2467,84 @@
   </si>
   <si>
     <t>MANOJ.S</t>
+  </si>
+  <si>
+    <t>R.M. DHRUVIK</t>
+  </si>
+  <si>
+    <t>R.CHAITANYA</t>
+  </si>
+  <si>
+    <t>M.PRANAV</t>
+  </si>
+  <si>
+    <t>R.RIHAN</t>
+  </si>
+  <si>
+    <t>V.KASHVI</t>
+  </si>
+  <si>
+    <t>G.MOKSHA SRI</t>
+  </si>
+  <si>
+    <t>S.MAHAMMD ALMAS</t>
+  </si>
+  <si>
+    <t>P.MADHU SRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.VISHNU </t>
+  </si>
+  <si>
+    <t>R.V. DELWIN RAJ</t>
+  </si>
+  <si>
+    <t>A.B. YOSHITHA(DROP)</t>
+  </si>
+  <si>
+    <t>M.STALIN</t>
+  </si>
+  <si>
+    <t>S.HUMAYUN</t>
+  </si>
+  <si>
+    <t>V.MAGI</t>
+  </si>
+  <si>
+    <t>G.KIRAN</t>
+  </si>
+  <si>
+    <t>S.SHAMU</t>
+  </si>
+  <si>
+    <t>P VIJAY KUMAR</t>
+  </si>
+  <si>
+    <t>P SURESH</t>
+  </si>
+  <si>
+    <t>M.RAJASEKHAR</t>
+  </si>
+  <si>
+    <t>A.BASKAR</t>
+  </si>
+  <si>
+    <t>RAJULAKANDRIGA (HW)</t>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>LKG</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
+  </si>
+  <si>
+    <t>Getdate()</t>
+  </si>
+  <si>
+    <t>Purushotham</t>
   </si>
 </sst>
 </file>
@@ -2623,7 +2702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2761,6 +2840,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2775,20 +2869,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3096,7 +3181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3106,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4192,8 +4277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7594,19 +7679,19 @@
       <c r="A49" s="50" t="s">
         <v>742</v>
       </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="52"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="53"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="55"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="60"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
@@ -14522,19 +14607,19 @@
       <c r="A619" s="50" t="s">
         <v>753</v>
       </c>
-      <c r="B619" s="56"/>
-      <c r="C619" s="56"/>
-      <c r="D619" s="56"/>
-      <c r="E619" s="56"/>
-      <c r="F619" s="57"/>
+      <c r="B619" s="51"/>
+      <c r="C619" s="51"/>
+      <c r="D619" s="51"/>
+      <c r="E619" s="51"/>
+      <c r="F619" s="52"/>
     </row>
     <row r="620" spans="1:6">
-      <c r="A620" s="58"/>
-      <c r="B620" s="59"/>
-      <c r="C620" s="59"/>
-      <c r="D620" s="59"/>
-      <c r="E620" s="59"/>
-      <c r="F620" s="60"/>
+      <c r="A620" s="53"/>
+      <c r="B620" s="54"/>
+      <c r="C620" s="54"/>
+      <c r="D620" s="54"/>
+      <c r="E620" s="54"/>
+      <c r="F620" s="55"/>
     </row>
     <row r="621" spans="1:6">
       <c r="A621" s="1" t="s">
@@ -14736,6 +14821,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:F5"/>
+    <mergeCell ref="A96:F97"/>
+    <mergeCell ref="A146:F147"/>
+    <mergeCell ref="A196:F197"/>
+    <mergeCell ref="A245:F246"/>
+    <mergeCell ref="A49:F50"/>
     <mergeCell ref="A590:F591"/>
     <mergeCell ref="A619:F620"/>
     <mergeCell ref="A295:F296"/>
@@ -14744,15 +14835,467 @@
     <mergeCell ref="A441:F442"/>
     <mergeCell ref="A491:F492"/>
     <mergeCell ref="A540:F541"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="A96:F97"/>
-    <mergeCell ref="A146:F147"/>
-    <mergeCell ref="A196:F197"/>
-    <mergeCell ref="A245:F246"/>
-    <mergeCell ref="A49:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="171.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="3" customFormat="1">
+      <c r="A1" s="41" t="s">
+        <v>763</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>764</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>765</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>766</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>767</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>768</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>769</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>770</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>771</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>772</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>773</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>774</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>775</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>776</v>
+      </c>
+      <c r="O1" s="41"/>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1">
+      <c r="A2" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="3" customFormat="1">
+      <c r="A3" s="19" t="s">
+        <v>758</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>655</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="3" customFormat="1">
+      <c r="A4" s="19" t="s">
+        <v>761</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>762</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="3" customFormat="1">
+      <c r="A5" s="19" t="s">
+        <v>806</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>757</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="3" customFormat="1">
+      <c r="A6" s="19" t="s">
+        <v>807</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>816</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="3" customFormat="1">
+      <c r="A7" s="19" t="s">
+        <v>808</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="3" customFormat="1">
+      <c r="A8" s="19" t="s">
+        <v>809</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="3" customFormat="1">
+      <c r="A9" s="19" t="s">
+        <v>810</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>819</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="3" customFormat="1">
+      <c r="A10" s="19" t="s">
+        <v>759</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>760</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="3" customFormat="1">
+      <c r="A11" s="19" t="s">
+        <v>811</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>820</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="3" customFormat="1">
+      <c r="A12" s="19" t="s">
+        <v>812</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>821</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="3" customFormat="1">
+      <c r="A13" s="19" t="s">
+        <v>813</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="3" customFormat="1">
+      <c r="A14" s="19" t="s">
+        <v>814</v>
+      </c>
+      <c r="C14" s="9">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>823</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="3" customFormat="1">
+      <c r="A15" s="61" t="s">
+        <v>815</v>
+      </c>
+      <c r="C15" s="9">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="I15" s="61" t="s">
+        <v>824</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>